<commit_message>
Revertir al estado anterior sin eliminar historial
</commit_message>
<xml_diff>
--- a/app/tables/tabla_gaussSeidel.xlsx
+++ b/app/tables/tabla_gaussSeidel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,12 +458,114 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[0.5;0;1.33333333333333]</t>
+          <t>[1.66666666666667;1.08333333333333]</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>1.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>[1.30555555555556;1.17361111111111]</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0.276595744680851</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>[1.27546296296296;1.18113425925926]</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0.0235934664246824</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>[1.27295524691358;1.18176118827161]</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0.0019699954538566</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>[1.27274627057613;1.18181343235597]</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0.0001641932428166</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>[1.27272885588134;1.18181778602966]</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>1.36829574554376e-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>[1.27272740465678;1.18181814883581]</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1.1402477547978e-06</t>
         </is>
       </c>
     </row>

</xml_diff>